<commit_message>
update OBD-II connector info.
</commit_message>
<xml_diff>
--- a/electrical/sources/vehicle-interface.bom.xlsx
+++ b/electrical/sources/vehicle-interface.bom.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="40" windowWidth="23900" windowHeight="14960"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="23895" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="PartsList" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="LITEPOINT_TB">#REF!</definedName>
     <definedName name="Views">[1]Sheet2!$S$1:$S$9</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="286">
   <si>
     <t>Part</t>
   </si>
@@ -873,6 +873,18 @@
   </si>
   <si>
     <t>http://ca.mouser.com/Search/ProductDetail.aspx?qs=q1%252b4sgCmzzlrhULyC%252brCPA==</t>
+  </si>
+  <si>
+    <t>Comtech</t>
+  </si>
+  <si>
+    <t>http://www.cct-elec.com/sdp/213844/4/pd-955932/10065677-2539664/OBDII_16P_MRight_Angle_CONNECTOR.html</t>
+  </si>
+  <si>
+    <t>XK144220</t>
+  </si>
+  <si>
+    <t>30V</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1031,9 +1043,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,7 +1090,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1430,26 +1439,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="65.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5" style="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1490,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="24">
+    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="24">
+    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1539,7 +1548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="24">
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="24">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1600,7 +1609,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="24">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="24">
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1664,7 +1673,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="24">
+    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -1725,7 +1734,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="24">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -1757,7 +1766,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="24">
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>56</v>
       </c>
@@ -1786,7 +1795,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="24">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
@@ -1815,7 +1824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="24">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
@@ -1844,7 +1853,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="24">
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
@@ -1873,7 +1882,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="36">
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>81</v>
       </c>
@@ -1902,7 +1911,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="24">
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>87</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="24">
+    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>94</v>
       </c>
@@ -1960,7 +1969,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="36">
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>101</v>
       </c>
@@ -1989,7 +1998,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="36">
+    <row r="19" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>107</v>
       </c>
@@ -2018,7 +2027,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="24">
+    <row r="20" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>114</v>
       </c>
@@ -2047,7 +2056,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="36">
+    <row r="21" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>120</v>
       </c>
@@ -2076,7 +2085,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="24">
+    <row r="22" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>126</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="24">
+    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>131</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="24">
+    <row r="24" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>136</v>
       </c>
@@ -2163,7 +2172,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="24">
+    <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>143</v>
       </c>
@@ -2192,7 +2201,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>149</v>
       </c>
@@ -2205,13 +2214,23 @@
       <c r="D26" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" ht="36">
+      <c r="E26" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>152</v>
       </c>
@@ -2240,7 +2259,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="24">
+    <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>158</v>
       </c>
@@ -2269,7 +2288,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="24">
+    <row r="29" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>164</v>
       </c>
@@ -2294,7 +2313,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="24">
+    <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>170</v>
       </c>
@@ -2323,7 +2342,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="24">
+    <row r="31" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>176</v>
       </c>
@@ -2352,7 +2371,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="24">
+    <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>183</v>
       </c>
@@ -2381,7 +2400,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="36">
+    <row r="33" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>191</v>
       </c>
@@ -2410,7 +2429,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="24">
+    <row r="34" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>198</v>
       </c>
@@ -2439,7 +2458,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="24">
+    <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>205</v>
       </c>
@@ -2468,7 +2487,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="36">
+    <row r="36" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>212</v>
       </c>
@@ -2500,7 +2519,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="36">
+    <row r="37" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>218</v>
       </c>
@@ -2532,7 +2551,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="36">
+    <row r="38" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>222</v>
       </c>
@@ -2564,7 +2583,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="36">
+    <row r="39" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>226</v>
       </c>
@@ -2596,7 +2615,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>230</v>
       </c>
@@ -2609,23 +2628,23 @@
       <c r="D40" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H40" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="I40" s="14" t="s">
+      <c r="I40" s="13" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="36">
+    <row r="41" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>234</v>
       </c>
@@ -2657,7 +2676,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="36">
+    <row r="42" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>237</v>
       </c>
@@ -2689,7 +2708,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="36">
+    <row r="43" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>240</v>
       </c>
@@ -2721,7 +2740,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="36">
+    <row r="44" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>243</v>
       </c>
@@ -2753,7 +2772,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="36">
+    <row r="45" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>247</v>
       </c>
@@ -2785,7 +2804,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="36">
+    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>251</v>
       </c>
@@ -2817,7 +2836,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="24">
+    <row r="47" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>255</v>
       </c>
@@ -2846,7 +2865,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="33.75" customHeight="1"/>
+    <row r="48" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
@@ -2892,6 +2911,7 @@
     <hyperlink ref="I45" r:id="rId40"/>
     <hyperlink ref="I46" r:id="rId41"/>
     <hyperlink ref="I47" r:id="rId42"/>
+    <hyperlink ref="I26" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>